<commit_message>
modified graphs to improve visiblity in paper
</commit_message>
<xml_diff>
--- a/experimental_data_collection/validation.xlsx
+++ b/experimental_data_collection/validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceccarelli/Google Drive/REU/REU-Drone-Swarm-Optimization/experimental_data_collection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceccarelli/Google Drive/Old/REU Summer 2019/REU-Drone-Swarm-Optimization/experimental_data_collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84625AB-3FBC-B947-9E5C-B21A403F653B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8984A27-9D14-B845-8FD1-F77A978CCA30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" firstSheet="3" activeTab="9" xr2:uid="{D9324A89-EF1B-2742-8BF0-637F7EBB650A}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" firstSheet="4" activeTab="9" xr2:uid="{D9324A89-EF1B-2742-8BF0-637F7EBB650A}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Size" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="78">
   <si>
     <t>Population Size</t>
   </si>
@@ -369,6 +370,12 @@
   <si>
     <t>&lt;-- poster graphs</t>
   </si>
+  <si>
+    <t>Fig 5.  Fitness Function and Natural</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Selection Method Evaluation Data</t>
+  </si>
 </sst>
 </file>
 
@@ -667,7 +674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -783,6 +790,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2737,7 +2747,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -2747,7 +2757,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
+              <a:rPr lang="en-US" sz="1300"/>
               <a:t>Runtime of Proposed Algorithm with Different Fitness Functions </a:t>
             </a:r>
           </a:p>
@@ -2766,7 +2776,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -3134,7 +3144,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1300"/>
               <a:t>User Coverage of Proposed Algorithm with Different Fitness Functions</a:t>
             </a:r>
           </a:p>
@@ -3512,7 +3522,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -3522,7 +3532,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1300"/>
               <a:t>Number of UAVs Used by Proposed Algorithm with Different Fitness Functions</a:t>
             </a:r>
           </a:p>
@@ -3541,7 +3551,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -3909,7 +3919,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1300"/>
               <a:t>Runtime of Proposed Algorithm with Different Natural Selection Methods</a:t>
             </a:r>
           </a:p>
@@ -4280,7 +4290,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -4290,7 +4300,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1300"/>
               <a:t>Number of UAVs used by Proposed Algorithm with Different Natural Selection Methods</a:t>
             </a:r>
           </a:p>
@@ -4309,7 +4319,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -23467,13 +23477,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>815340</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>11239</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23502,16 +23512,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>821872</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1429</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>811712</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>11239</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23540,16 +23550,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>821872</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1429</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>811712</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>44956</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23578,16 +23588,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>7265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>802640</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>810694</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>191062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23616,16 +23626,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>804793</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>817945</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>21903</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>794633</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>807785</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>11239</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23660,15 +23670,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>131761</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>150019</xdr:rowOff>
+      <xdr:colOff>24134</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>10104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>788717</xdr:colOff>
+      <xdr:colOff>681090</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>91282</xdr:rowOff>
+      <xdr:rowOff>155858</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23697,16 +23707,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>828728</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>157955</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>10762</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>7277</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>656955</xdr:colOff>
+      <xdr:colOff>667718</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>107156</xdr:rowOff>
+      <xdr:rowOff>160969</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -24596,8 +24606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC1CC26-8D99-9045-B928-93174DC11408}">
   <dimension ref="B2:BD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I25" zoomScale="118" workbookViewId="0">
-      <selection activeCell="U45" sqref="U45"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="118" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29368,15 +29378,40 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C483DB58-05D7-DD45-AD01-FB1A8995E4AA}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="I15:L16"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView zoomScale="113" workbookViewId="0">
+      <selection activeCell="L20" sqref="A1:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="15" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I15" s="92" t="s">
+        <v>76</v>
+      </c>
+      <c r="J15" s="92"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="92"/>
+    </row>
+    <row r="16" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I16" s="92" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="92"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="89" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>